<commit_message>
Final Push with annotation and some changers
</commit_message>
<xml_diff>
--- a/DotNet/wwwroot/Uploads/data.xlsx
+++ b/DotNet/wwwroot/Uploads/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F36D01F-BE67-41BE-98A4-CC8CE3FE1C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1041BE14-2DB9-4B0E-AA6C-DB6D88573207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Serial No</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Food</t>
-  </si>
-  <si>
-    <t>Tech</t>
-  </si>
-  <si>
     <t>Cloth</t>
   </si>
   <si>
@@ -61,6 +55,42 @@
   </si>
   <si>
     <t>Fish</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Egg</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Deo</t>
+  </si>
+  <si>
+    <t>Islamic</t>
+  </si>
+  <si>
+    <t>Sad</t>
+  </si>
+  <si>
+    <t>Happy</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Ram</t>
   </si>
 </sst>
 </file>
@@ -378,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +429,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -407,7 +437,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -415,7 +445,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -423,7 +453,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -431,7 +461,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -439,7 +469,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -447,7 +477,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -455,7 +485,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -463,7 +493,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -471,7 +501,87 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>